<commit_message>
add balanced distance result
</commit_message>
<xml_diff>
--- a/fs_results.xlsx
+++ b/fs_results.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuchen.zhang/Documents/Projects/domain-adaptation-nlp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02252B9C-9276-A04C-9EE4-7C8B0D449A18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732409A0-0E89-6D44-9F17-53A9723D6D18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{142A77BE-4AFC-3D4B-A91F-57D86A919EE1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{142A77BE-4AFC-3D4B-A91F-57D86A919EE1}"/>
   </bookViews>
   <sheets>
-    <sheet name="conf_lm" sheetId="2" r:id="rId1"/>
-    <sheet name="conf_lm_T" sheetId="3" r:id="rId2"/>
-    <sheet name="vanila_distance_lm" sheetId="1" r:id="rId3"/>
+    <sheet name="conf_lm_t" sheetId="4" r:id="rId1"/>
+    <sheet name="conf_lm_t_transpose" sheetId="5" r:id="rId2"/>
+    <sheet name="conf_lm" sheetId="2" r:id="rId3"/>
+    <sheet name="conf_lm_transpose" sheetId="3" r:id="rId4"/>
+    <sheet name="vanila_distance_lm" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="41">
   <si>
     <t>Home_and_Kitchen.train_to_Home_and_Kitchen.train</t>
   </si>
@@ -156,6 +158,9 @@
   </si>
   <si>
     <t>DVDs</t>
+  </si>
+  <si>
+    <t>num_iter</t>
   </si>
 </sst>
 </file>
@@ -324,7 +329,1255 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="304">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -944,7 +2197,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$A$3:$Q$29" spid="_x0000_s1162"/>
+                  <a14:cameraTool cellRange="$A$3:$Q$29" spid="_x0000_s1183"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1280,11 +2533,2850 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F5B09C-0900-3442-A427-C6977CDBA906}">
+  <dimension ref="A1:R30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:R24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" style="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="17" t="str">
+        <f>SUBSTITUTE(LEFT(C$1,FIND(".train_to_",C$1)-1),"_"," ")</f>
+        <v>Home and Kitchen</v>
+      </c>
+      <c r="D2" s="17" t="str">
+        <f t="shared" ref="D2:R2" si="0">SUBSTITUTE(LEFT(D$1,FIND(".train_to_",D$1)-1),"_"," ")</f>
+        <v>Home and Kitchen</v>
+      </c>
+      <c r="E2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Home and Kitchen</v>
+      </c>
+      <c r="F2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Home and Kitchen</v>
+      </c>
+      <c r="G2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Movies and TV</v>
+      </c>
+      <c r="H2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Movies and TV</v>
+      </c>
+      <c r="I2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Movies and TV</v>
+      </c>
+      <c r="J2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Movies and TV</v>
+      </c>
+      <c r="K2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Electronics</v>
+      </c>
+      <c r="L2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Electronics</v>
+      </c>
+      <c r="M2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Electronics</v>
+      </c>
+      <c r="N2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Electronics</v>
+      </c>
+      <c r="O2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Books</v>
+      </c>
+      <c r="P2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Books</v>
+      </c>
+      <c r="Q2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Books</v>
+      </c>
+      <c r="R2" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>Books</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="17" t="str">
+        <f>SUBSTITUTE(MID(C$1,FIND("_to_",C$1)+4,LEN(C$1) -(FIND("_to_",C$1)+9)), "_"," ")</f>
+        <v>Home and Kitchen</v>
+      </c>
+      <c r="D3" s="17" t="str">
+        <f t="shared" ref="D3:R3" si="1">SUBSTITUTE(MID(D$1,FIND("_to_",D$1)+4,LEN(D$1) -(FIND("_to_",D$1)+9)), "_"," ")</f>
+        <v>Movies and TV</v>
+      </c>
+      <c r="E3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Electronics</v>
+      </c>
+      <c r="F3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Books</v>
+      </c>
+      <c r="G3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Home and Kitchen</v>
+      </c>
+      <c r="H3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Movies and TV</v>
+      </c>
+      <c r="I3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Electronics</v>
+      </c>
+      <c r="J3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Books</v>
+      </c>
+      <c r="K3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Home and Kitchen</v>
+      </c>
+      <c r="L3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Movies and TV</v>
+      </c>
+      <c r="M3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Electronics</v>
+      </c>
+      <c r="N3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Books</v>
+      </c>
+      <c r="O3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Home and Kitchen</v>
+      </c>
+      <c r="P3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Movies and TV</v>
+      </c>
+      <c r="Q3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Electronics</v>
+      </c>
+      <c r="R3" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Books</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="21">
+        <v>0.93</v>
+      </c>
+      <c r="D6" s="21">
+        <v>0.93</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0.93</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0.93</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="I6" s="21">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="J6" s="21">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="L6" s="21">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="M6" s="21">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="N6" s="21">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="O6" s="21">
+        <v>0.9415</v>
+      </c>
+      <c r="P6" s="21">
+        <v>0.9415</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>0.9415</v>
+      </c>
+      <c r="R6" s="21">
+        <v>0.9415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="21">
+        <v>0.93</v>
+      </c>
+      <c r="D7" s="21">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="E7" s="21">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="F7" s="21">
+        <v>0.9415</v>
+      </c>
+      <c r="G7" s="21">
+        <v>0.93</v>
+      </c>
+      <c r="H7" s="21">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="I7" s="21">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="J7" s="21">
+        <v>0.9415</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0.93</v>
+      </c>
+      <c r="L7" s="21">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="M7" s="21">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="N7" s="21">
+        <v>0.9415</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0.93</v>
+      </c>
+      <c r="P7" s="21">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="R7" s="21">
+        <v>0.9415</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.878</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="F9" s="23">
+        <v>0.89649999999999996</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="H9" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="I9" s="23">
+        <v>0.8155</v>
+      </c>
+      <c r="J9" s="23">
+        <v>0.91649999999999998</v>
+      </c>
+      <c r="K9" s="23">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="L9" s="23">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="M9" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="N9" s="23">
+        <v>0.89249999999999996</v>
+      </c>
+      <c r="O9" s="23">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="P9" s="23">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="Q9" s="23">
+        <v>0.80449999999999999</v>
+      </c>
+      <c r="R9" s="23">
+        <v>0.9415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="D10" s="23">
+        <v>0.877</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="F10" s="23">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0.87250000000000005</v>
+      </c>
+      <c r="H10" s="23">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="I10" s="23">
+        <v>0.81</v>
+      </c>
+      <c r="J10" s="23">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="K10" s="23">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="L10" s="23">
+        <v>0.90649999999999997</v>
+      </c>
+      <c r="M10" s="23">
+        <v>0.91549999999999998</v>
+      </c>
+      <c r="N10" s="23">
+        <v>0.90049999999999997</v>
+      </c>
+      <c r="O10" s="23">
+        <v>0.84950000000000003</v>
+      </c>
+      <c r="P10" s="23">
+        <v>0.90349999999999997</v>
+      </c>
+      <c r="Q10" s="23">
+        <v>0.80549999999999999</v>
+      </c>
+      <c r="R10" s="23">
+        <v>0.9415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="23">
+        <v>0.92549999999999999</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0.90349999999999997</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.89949999999999997</v>
+      </c>
+      <c r="F11" s="23">
+        <v>0.91449999999999998</v>
+      </c>
+      <c r="G11" s="23">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="H11" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="I11" s="23">
+        <v>0.89049999999999996</v>
+      </c>
+      <c r="J11" s="23">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="K11" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="L11" s="23">
+        <v>0.91</v>
+      </c>
+      <c r="M11" s="23">
+        <v>0.91049999999999998</v>
+      </c>
+      <c r="N11" s="23">
+        <v>0.91849999999999998</v>
+      </c>
+      <c r="O11" s="23">
+        <v>0.88849999999999996</v>
+      </c>
+      <c r="P11" s="23">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="Q11" s="23">
+        <v>0.879</v>
+      </c>
+      <c r="R11" s="23">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="27">
+        <v>12</v>
+      </c>
+      <c r="D12" s="27">
+        <v>13</v>
+      </c>
+      <c r="E12" s="27">
+        <v>14</v>
+      </c>
+      <c r="F12" s="27">
+        <v>13</v>
+      </c>
+      <c r="G12" s="27">
+        <v>14</v>
+      </c>
+      <c r="H12" s="27">
+        <v>12</v>
+      </c>
+      <c r="I12" s="27">
+        <v>13</v>
+      </c>
+      <c r="J12" s="27">
+        <v>15</v>
+      </c>
+      <c r="K12" s="27">
+        <v>13</v>
+      </c>
+      <c r="L12" s="27">
+        <v>13</v>
+      </c>
+      <c r="M12" s="27">
+        <v>12</v>
+      </c>
+      <c r="N12" s="27">
+        <v>13</v>
+      </c>
+      <c r="O12" s="27">
+        <v>14</v>
+      </c>
+      <c r="P12" s="27">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="27">
+        <v>18</v>
+      </c>
+      <c r="R12" s="27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="23">
+        <v>0.93004500000000001</v>
+      </c>
+      <c r="D14" s="23">
+        <v>0.90135900000000002</v>
+      </c>
+      <c r="E14" s="23">
+        <v>0.887714</v>
+      </c>
+      <c r="F14" s="23">
+        <v>0.898339</v>
+      </c>
+      <c r="G14" s="23">
+        <v>0.88463499999999995</v>
+      </c>
+      <c r="H14" s="23">
+        <v>0.92601900000000004</v>
+      </c>
+      <c r="I14" s="23">
+        <v>0.84750899999999996</v>
+      </c>
+      <c r="J14" s="23">
+        <v>0.91481900000000005</v>
+      </c>
+      <c r="K14" s="23">
+        <v>0.91641499999999998</v>
+      </c>
+      <c r="L14" s="23">
+        <v>0.900756</v>
+      </c>
+      <c r="M14" s="23">
+        <v>0.91444400000000003</v>
+      </c>
+      <c r="N14" s="23">
+        <v>0.88525399999999999</v>
+      </c>
+      <c r="O14" s="23">
+        <v>0.87361500000000003</v>
+      </c>
+      <c r="P14" s="23">
+        <v>0.90529000000000004</v>
+      </c>
+      <c r="Q14" s="23">
+        <v>0.86074700000000004</v>
+      </c>
+      <c r="R14" s="23">
+        <v>0.94114699999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="23">
+        <v>0.92954199999999998</v>
+      </c>
+      <c r="D15" s="23">
+        <v>0.88173100000000004</v>
+      </c>
+      <c r="E15" s="23">
+        <v>0.88570000000000004</v>
+      </c>
+      <c r="F15" s="23">
+        <v>0.89431300000000002</v>
+      </c>
+      <c r="G15" s="23">
+        <v>0.87607100000000004</v>
+      </c>
+      <c r="H15" s="23">
+        <v>0.92551600000000001</v>
+      </c>
+      <c r="I15" s="23">
+        <v>0.82687500000000003</v>
+      </c>
+      <c r="J15" s="23">
+        <v>0.91885099999999997</v>
+      </c>
+      <c r="K15" s="23">
+        <v>0.91742199999999996</v>
+      </c>
+      <c r="L15" s="23">
+        <v>0.90115999999999996</v>
+      </c>
+      <c r="M15" s="23">
+        <v>0.91494699999999995</v>
+      </c>
+      <c r="N15" s="23">
+        <v>0.89380999999999999</v>
+      </c>
+      <c r="O15" s="23">
+        <v>0.86656599999999995</v>
+      </c>
+      <c r="P15" s="23">
+        <v>0.90327500000000005</v>
+      </c>
+      <c r="Q15" s="23">
+        <v>0.83299699999999999</v>
+      </c>
+      <c r="R15" s="23">
+        <v>0.94064400000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="23">
+        <v>0.93407099999999998</v>
+      </c>
+      <c r="D16" s="23">
+        <v>0.89783599999999997</v>
+      </c>
+      <c r="E16" s="23">
+        <v>0.88922500000000004</v>
+      </c>
+      <c r="F16" s="23">
+        <v>0.89330600000000004</v>
+      </c>
+      <c r="G16" s="23">
+        <v>0.88161199999999995</v>
+      </c>
+      <c r="H16" s="23">
+        <v>0.928535</v>
+      </c>
+      <c r="I16" s="23">
+        <v>0.85707100000000003</v>
+      </c>
+      <c r="J16" s="23">
+        <v>0.92691500000000004</v>
+      </c>
+      <c r="K16" s="23">
+        <v>0.918933</v>
+      </c>
+      <c r="L16" s="23">
+        <v>0.90267299999999995</v>
+      </c>
+      <c r="M16" s="23">
+        <v>0.91595400000000005</v>
+      </c>
+      <c r="N16" s="23">
+        <v>0.90286900000000003</v>
+      </c>
+      <c r="O16" s="23">
+        <v>0.86807699999999999</v>
+      </c>
+      <c r="P16" s="23">
+        <v>0.91335</v>
+      </c>
+      <c r="Q16" s="23">
+        <v>0.86831499999999995</v>
+      </c>
+      <c r="R16" s="23">
+        <v>0.94315899999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="23">
+        <v>0.92652199999999996</v>
+      </c>
+      <c r="D17" s="23">
+        <v>0.90488199999999996</v>
+      </c>
+      <c r="E17" s="23">
+        <v>0.89627400000000002</v>
+      </c>
+      <c r="F17" s="23">
+        <v>0.913941</v>
+      </c>
+      <c r="G17" s="23">
+        <v>0.89168800000000004</v>
+      </c>
+      <c r="H17" s="23">
+        <v>0.92551600000000001</v>
+      </c>
+      <c r="I17" s="23">
+        <v>0.88927999999999996</v>
+      </c>
+      <c r="J17" s="23">
+        <v>0.92288300000000001</v>
+      </c>
+      <c r="K17" s="23">
+        <v>0.91641499999999998</v>
+      </c>
+      <c r="L17" s="23">
+        <v>0.90932000000000002</v>
+      </c>
+      <c r="M17" s="23">
+        <v>0.91041799999999995</v>
+      </c>
+      <c r="N17" s="23">
+        <v>0.91897300000000004</v>
+      </c>
+      <c r="O17" s="23">
+        <v>0.88922500000000004</v>
+      </c>
+      <c r="P17" s="23">
+        <v>0.91133500000000001</v>
+      </c>
+      <c r="Q17" s="23">
+        <v>0.87790100000000004</v>
+      </c>
+      <c r="R17" s="23">
+        <v>0.940141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="21">
+        <v>13</v>
+      </c>
+      <c r="D18" s="21">
+        <v>13</v>
+      </c>
+      <c r="E18" s="21">
+        <v>14</v>
+      </c>
+      <c r="F18" s="21">
+        <v>13</v>
+      </c>
+      <c r="G18" s="21">
+        <v>15</v>
+      </c>
+      <c r="H18" s="21">
+        <v>13</v>
+      </c>
+      <c r="I18" s="21">
+        <v>13</v>
+      </c>
+      <c r="J18" s="21">
+        <v>16</v>
+      </c>
+      <c r="K18" s="21">
+        <v>14</v>
+      </c>
+      <c r="L18" s="21">
+        <v>17</v>
+      </c>
+      <c r="M18" s="21">
+        <v>13</v>
+      </c>
+      <c r="N18" s="21">
+        <v>13</v>
+      </c>
+      <c r="O18" s="21">
+        <v>14</v>
+      </c>
+      <c r="P18" s="21">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>18</v>
+      </c>
+      <c r="R18" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B20" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="23">
+        <v>0.92857100000000004</v>
+      </c>
+      <c r="D20" s="23">
+        <v>0.89778400000000003</v>
+      </c>
+      <c r="E20" s="23">
+        <v>0.887714</v>
+      </c>
+      <c r="F20" s="23">
+        <v>0.897281</v>
+      </c>
+      <c r="G20" s="23">
+        <v>0.88318200000000002</v>
+      </c>
+      <c r="H20" s="23">
+        <v>0.92605599999999999</v>
+      </c>
+      <c r="I20" s="23">
+        <v>0.86448400000000003</v>
+      </c>
+      <c r="J20" s="23">
+        <v>0.915493</v>
+      </c>
+      <c r="K20" s="23">
+        <v>0.91586900000000004</v>
+      </c>
+      <c r="L20" s="23">
+        <v>0.90478599999999998</v>
+      </c>
+      <c r="M20" s="23">
+        <v>0.91490400000000005</v>
+      </c>
+      <c r="N20" s="23">
+        <v>0.89034199999999997</v>
+      </c>
+      <c r="O20" s="23">
+        <v>0.87663599999999997</v>
+      </c>
+      <c r="P20" s="23">
+        <v>0.90922800000000004</v>
+      </c>
+      <c r="Q20" s="23">
+        <v>0.84793600000000002</v>
+      </c>
+      <c r="R20" s="23">
+        <v>0.94114699999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B21" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="23">
+        <v>0.93008000000000002</v>
+      </c>
+      <c r="D21" s="23">
+        <v>0.89017599999999997</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0.88872099999999998</v>
+      </c>
+      <c r="F21" s="23">
+        <v>0.89521399999999995</v>
+      </c>
+      <c r="G21" s="23">
+        <v>0.884189</v>
+      </c>
+      <c r="H21" s="23">
+        <v>0.92555299999999996</v>
+      </c>
+      <c r="I21" s="23">
+        <v>0.84282100000000004</v>
+      </c>
+      <c r="J21" s="23">
+        <v>0.91998000000000002</v>
+      </c>
+      <c r="K21" s="23">
+        <v>0.91885099999999997</v>
+      </c>
+      <c r="L21" s="23">
+        <v>0.90221799999999996</v>
+      </c>
+      <c r="M21" s="23">
+        <v>0.915408</v>
+      </c>
+      <c r="N21" s="23">
+        <v>0.89738399999999996</v>
+      </c>
+      <c r="O21" s="23">
+        <v>0.86448400000000003</v>
+      </c>
+      <c r="P21" s="23">
+        <v>0.90317700000000001</v>
+      </c>
+      <c r="Q21" s="23">
+        <v>0.81218500000000005</v>
+      </c>
+      <c r="R21" s="23">
+        <v>0.94114699999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B22" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="23">
+        <v>0.93360200000000004</v>
+      </c>
+      <c r="D22" s="23">
+        <v>0.89622199999999996</v>
+      </c>
+      <c r="E22" s="23">
+        <v>0.88922500000000004</v>
+      </c>
+      <c r="F22" s="23">
+        <v>0.89420699999999997</v>
+      </c>
+      <c r="G22" s="23">
+        <v>0.88368599999999997</v>
+      </c>
+      <c r="H22" s="23">
+        <v>0.928068</v>
+      </c>
+      <c r="I22" s="23">
+        <v>0.85743100000000005</v>
+      </c>
+      <c r="J22" s="23">
+        <v>0.92652199999999996</v>
+      </c>
+      <c r="K22" s="23">
+        <v>0.91985899999999998</v>
+      </c>
+      <c r="L22" s="23">
+        <v>0.89868999999999999</v>
+      </c>
+      <c r="M22" s="23">
+        <v>0.91591100000000003</v>
+      </c>
+      <c r="N22" s="23">
+        <v>0.90040200000000004</v>
+      </c>
+      <c r="O22" s="23">
+        <v>0.86952099999999999</v>
+      </c>
+      <c r="P22" s="23">
+        <v>0.913767</v>
+      </c>
+      <c r="Q22" s="23">
+        <v>0.85901300000000003</v>
+      </c>
+      <c r="R22" s="23">
+        <v>0.94315899999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B23" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="23">
+        <v>0.92605599999999999</v>
+      </c>
+      <c r="D23" s="23">
+        <v>0.90281999999999996</v>
+      </c>
+      <c r="E23" s="23">
+        <v>0.89879200000000004</v>
+      </c>
+      <c r="F23" s="23">
+        <v>0.915408</v>
+      </c>
+      <c r="G23" s="23">
+        <v>0.89174200000000003</v>
+      </c>
+      <c r="H23" s="23">
+        <v>0.92605599999999999</v>
+      </c>
+      <c r="I23" s="23">
+        <v>0.89017599999999997</v>
+      </c>
+      <c r="J23" s="23">
+        <v>0.92253499999999999</v>
+      </c>
+      <c r="K23" s="23">
+        <v>0.91536499999999998</v>
+      </c>
+      <c r="L23" s="23">
+        <v>0.91234300000000002</v>
+      </c>
+      <c r="M23" s="23">
+        <v>0.91037299999999999</v>
+      </c>
+      <c r="N23" s="23">
+        <v>0.91851099999999997</v>
+      </c>
+      <c r="O23" s="23">
+        <v>0.89174200000000003</v>
+      </c>
+      <c r="P23" s="23">
+        <v>0.913767</v>
+      </c>
+      <c r="Q23" s="23">
+        <v>0.88217500000000004</v>
+      </c>
+      <c r="R23" s="23">
+        <v>0.93963799999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="21">
+        <v>12</v>
+      </c>
+      <c r="D24" s="21">
+        <v>15</v>
+      </c>
+      <c r="E24" s="21">
+        <v>14</v>
+      </c>
+      <c r="F24" s="21">
+        <v>15</v>
+      </c>
+      <c r="G24" s="21">
+        <v>14</v>
+      </c>
+      <c r="H24" s="21">
+        <v>12</v>
+      </c>
+      <c r="I24" s="21">
+        <v>15</v>
+      </c>
+      <c r="J24" s="21">
+        <v>13</v>
+      </c>
+      <c r="K24" s="21">
+        <v>16</v>
+      </c>
+      <c r="L24" s="21">
+        <v>16</v>
+      </c>
+      <c r="M24" s="21">
+        <v>14</v>
+      </c>
+      <c r="N24" s="21">
+        <v>12</v>
+      </c>
+      <c r="O24" s="21">
+        <v>15</v>
+      </c>
+      <c r="P24" s="21">
+        <v>17</v>
+      </c>
+      <c r="Q24" s="21">
+        <v>14</v>
+      </c>
+      <c r="R24" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B26" s="21">
+        <f>AVERAGE(C26:R26)</f>
+        <v>0.375</v>
+      </c>
+      <c r="C26">
+        <f>(C17&gt;C11)*1</f>
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:R26" si="2">(D17&gt;D11)*1</f>
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B27" s="21">
+        <f>AVERAGE(C27:R27)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C27">
+        <f>(C23&gt;C11)*1</f>
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ref="D27:R27" si="3">(D23&gt;D11)*1</f>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B28" s="21">
+        <f t="shared" ref="B28:B30" si="4">AVERAGE(C28:R28)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="C28">
+        <f>(C16&gt;C15)*1</f>
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ref="D28:R28" si="5">(D16&gt;D15)*1</f>
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B29" s="21">
+        <f t="shared" si="4"/>
+        <v>0.8125</v>
+      </c>
+      <c r="C29" s="29">
+        <f>(C22&gt;C21)*1</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="29">
+        <f t="shared" ref="D29:R29" si="6">(D22&gt;D21)*1</f>
+        <v>1</v>
+      </c>
+      <c r="E29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F29" s="29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L29" s="29">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="N29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="O29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="Q29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R29" s="29">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="21">
+        <f t="shared" si="4"/>
+        <v>0.5625</v>
+      </c>
+      <c r="C30" s="29">
+        <f>(C23&gt;C17)*1</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="29">
+        <f t="shared" ref="D30:R30" si="7">(D23&gt;D17)*1</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G30" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H30" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I30" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J30" s="29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="M30" s="29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P30" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q30" s="29">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="R30" s="29">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C14:C17">
+    <cfRule type="top10" dxfId="303" priority="48" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:D17">
+    <cfRule type="top10" dxfId="302" priority="47" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E17">
+    <cfRule type="top10" dxfId="301" priority="46" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:F17">
+    <cfRule type="top10" dxfId="300" priority="45" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14:G17">
+    <cfRule type="top10" dxfId="299" priority="44" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:H17">
+    <cfRule type="top10" dxfId="298" priority="43" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I17">
+    <cfRule type="top10" dxfId="297" priority="42" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14:J17">
+    <cfRule type="top10" dxfId="296" priority="41" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14:K17">
+    <cfRule type="top10" dxfId="295" priority="40" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14:L17">
+    <cfRule type="top10" dxfId="294" priority="39" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M14:M17">
+    <cfRule type="top10" dxfId="293" priority="38" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N14:N17">
+    <cfRule type="top10" dxfId="292" priority="37" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O14:O17">
+    <cfRule type="top10" dxfId="291" priority="36" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P14:P17">
+    <cfRule type="top10" dxfId="290" priority="35" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q14:Q17">
+    <cfRule type="top10" dxfId="289" priority="34" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R14:R17">
+    <cfRule type="top10" dxfId="288" priority="33" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:C23">
+    <cfRule type="top10" dxfId="287" priority="32" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:D23">
+    <cfRule type="top10" dxfId="286" priority="31" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E23">
+    <cfRule type="top10" dxfId="285" priority="30" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20:F23">
+    <cfRule type="top10" dxfId="284" priority="29" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20:G23">
+    <cfRule type="top10" dxfId="283" priority="28" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20:H23">
+    <cfRule type="top10" dxfId="282" priority="27" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I20:I23">
+    <cfRule type="top10" dxfId="281" priority="26" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J20:J23">
+    <cfRule type="top10" dxfId="280" priority="25" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20:K23">
+    <cfRule type="top10" dxfId="279" priority="24" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L20:L23">
+    <cfRule type="top10" dxfId="278" priority="23" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M20:M23">
+    <cfRule type="top10" dxfId="277" priority="22" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N20:N23">
+    <cfRule type="top10" dxfId="276" priority="21" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O20:O23">
+    <cfRule type="top10" dxfId="275" priority="20" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P20:P23">
+    <cfRule type="top10" dxfId="274" priority="19" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q20:Q23">
+    <cfRule type="top10" dxfId="273" priority="18" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R20:R23">
+    <cfRule type="top10" dxfId="272" priority="17" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:C11">
+    <cfRule type="top10" dxfId="271" priority="16" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:D11">
+    <cfRule type="top10" dxfId="270" priority="15" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E11">
+    <cfRule type="top10" dxfId="269" priority="14" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9:F11">
+    <cfRule type="top10" dxfId="268" priority="13" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9:G11">
+    <cfRule type="top10" dxfId="267" priority="12" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:H11">
+    <cfRule type="top10" dxfId="266" priority="11" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I11">
+    <cfRule type="top10" dxfId="265" priority="10" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9:J11">
+    <cfRule type="top10" dxfId="264" priority="9" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9:K11">
+    <cfRule type="top10" dxfId="263" priority="8" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:L11">
+    <cfRule type="top10" dxfId="262" priority="7" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M9:M11">
+    <cfRule type="top10" dxfId="261" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N9:N11">
+    <cfRule type="top10" dxfId="260" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O9:O11">
+    <cfRule type="top10" dxfId="259" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P9:P11">
+    <cfRule type="top10" dxfId="258" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q9:Q11">
+    <cfRule type="top10" dxfId="257" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R9:R11">
+    <cfRule type="top10" dxfId="256" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E34713E-696F-F445-AF06-5EDA0D7CC678}">
+  <dimension ref="A1:X18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="26"/>
+      <c r="M1" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="26"/>
+      <c r="S1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" s="26"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="X2" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="G3" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="J3" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="K3" s="23">
+        <v>0.92549999999999999</v>
+      </c>
+      <c r="L3" s="27">
+        <v>12</v>
+      </c>
+      <c r="M3" s="25"/>
+      <c r="N3" s="23">
+        <v>0.93004500000000001</v>
+      </c>
+      <c r="O3" s="23">
+        <v>0.92954199999999998</v>
+      </c>
+      <c r="P3" s="23">
+        <v>0.93407099999999998</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>0.92652199999999996</v>
+      </c>
+      <c r="R3" s="21">
+        <v>13</v>
+      </c>
+      <c r="S3" s="25"/>
+      <c r="T3" s="23">
+        <v>0.92857100000000004</v>
+      </c>
+      <c r="U3" s="23">
+        <v>0.93008000000000002</v>
+      </c>
+      <c r="V3" s="23">
+        <v>0.93360200000000004</v>
+      </c>
+      <c r="W3" s="23">
+        <v>0.92605599999999999</v>
+      </c>
+      <c r="X3" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="23">
+        <v>0.878</v>
+      </c>
+      <c r="J4" s="23">
+        <v>0.877</v>
+      </c>
+      <c r="K4" s="23">
+        <v>0.90349999999999997</v>
+      </c>
+      <c r="L4" s="27">
+        <v>13</v>
+      </c>
+      <c r="M4" s="25"/>
+      <c r="N4" s="23">
+        <v>0.90135900000000002</v>
+      </c>
+      <c r="O4" s="23">
+        <v>0.88173100000000004</v>
+      </c>
+      <c r="P4" s="23">
+        <v>0.89783599999999997</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>0.90488199999999996</v>
+      </c>
+      <c r="R4" s="21">
+        <v>13</v>
+      </c>
+      <c r="S4" s="25"/>
+      <c r="T4" s="23">
+        <v>0.89778400000000003</v>
+      </c>
+      <c r="U4" s="23">
+        <v>0.89017599999999997</v>
+      </c>
+      <c r="V4" s="23">
+        <v>0.89622199999999996</v>
+      </c>
+      <c r="W4" s="23">
+        <v>0.90281999999999996</v>
+      </c>
+      <c r="X4" s="21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="I5" s="23">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="J5" s="23">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="K5" s="23">
+        <v>0.89949999999999997</v>
+      </c>
+      <c r="L5" s="27">
+        <v>14</v>
+      </c>
+      <c r="M5" s="25"/>
+      <c r="N5" s="23">
+        <v>0.887714</v>
+      </c>
+      <c r="O5" s="23">
+        <v>0.88570000000000004</v>
+      </c>
+      <c r="P5" s="23">
+        <v>0.88922500000000004</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>0.89627400000000002</v>
+      </c>
+      <c r="R5" s="21">
+        <v>14</v>
+      </c>
+      <c r="S5" s="25"/>
+      <c r="T5" s="23">
+        <v>0.887714</v>
+      </c>
+      <c r="U5" s="23">
+        <v>0.88872099999999998</v>
+      </c>
+      <c r="V5" s="23">
+        <v>0.88922500000000004</v>
+      </c>
+      <c r="W5" s="23">
+        <v>0.89879200000000004</v>
+      </c>
+      <c r="X5" s="21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0.9415</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="I6" s="23">
+        <v>0.89649999999999996</v>
+      </c>
+      <c r="J6" s="23">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="K6" s="23">
+        <v>0.91449999999999998</v>
+      </c>
+      <c r="L6" s="27">
+        <v>13</v>
+      </c>
+      <c r="M6" s="25"/>
+      <c r="N6" s="23">
+        <v>0.898339</v>
+      </c>
+      <c r="O6" s="23">
+        <v>0.89431300000000002</v>
+      </c>
+      <c r="P6" s="23">
+        <v>0.89330600000000004</v>
+      </c>
+      <c r="Q6" s="23">
+        <v>0.913941</v>
+      </c>
+      <c r="R6" s="21">
+        <v>13</v>
+      </c>
+      <c r="S6" s="25"/>
+      <c r="T6" s="23">
+        <v>0.897281</v>
+      </c>
+      <c r="U6" s="23">
+        <v>0.89521399999999995</v>
+      </c>
+      <c r="V6" s="23">
+        <v>0.89420699999999997</v>
+      </c>
+      <c r="W6" s="23">
+        <v>0.915408</v>
+      </c>
+      <c r="X6" s="21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="G7" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="23">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="J7" s="23">
+        <v>0.87250000000000005</v>
+      </c>
+      <c r="K7" s="23">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="L7" s="27">
+        <v>14</v>
+      </c>
+      <c r="M7" s="25"/>
+      <c r="N7" s="23">
+        <v>0.88463499999999995</v>
+      </c>
+      <c r="O7" s="23">
+        <v>0.87607100000000004</v>
+      </c>
+      <c r="P7" s="23">
+        <v>0.88161199999999995</v>
+      </c>
+      <c r="Q7" s="23">
+        <v>0.89168800000000004</v>
+      </c>
+      <c r="R7" s="21">
+        <v>15</v>
+      </c>
+      <c r="S7" s="25"/>
+      <c r="T7" s="23">
+        <v>0.88318200000000002</v>
+      </c>
+      <c r="U7" s="23">
+        <v>0.884189</v>
+      </c>
+      <c r="V7" s="23">
+        <v>0.88368599999999997</v>
+      </c>
+      <c r="W7" s="23">
+        <v>0.89174200000000003</v>
+      </c>
+      <c r="X7" s="21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="J8" s="23">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="K8" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="L8" s="27">
+        <v>12</v>
+      </c>
+      <c r="M8" s="25"/>
+      <c r="N8" s="23">
+        <v>0.92601900000000004</v>
+      </c>
+      <c r="O8" s="23">
+        <v>0.92551600000000001</v>
+      </c>
+      <c r="P8" s="23">
+        <v>0.928535</v>
+      </c>
+      <c r="Q8" s="23">
+        <v>0.92551600000000001</v>
+      </c>
+      <c r="R8" s="21">
+        <v>13</v>
+      </c>
+      <c r="S8" s="25"/>
+      <c r="T8" s="23">
+        <v>0.92605599999999999</v>
+      </c>
+      <c r="U8" s="23">
+        <v>0.92555299999999996</v>
+      </c>
+      <c r="V8" s="23">
+        <v>0.928068</v>
+      </c>
+      <c r="W8" s="23">
+        <v>0.92605599999999999</v>
+      </c>
+      <c r="X8" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="H9" s="24"/>
+      <c r="I9" s="23">
+        <v>0.8155</v>
+      </c>
+      <c r="J9" s="23">
+        <v>0.81</v>
+      </c>
+      <c r="K9" s="23">
+        <v>0.89049999999999996</v>
+      </c>
+      <c r="L9" s="27">
+        <v>13</v>
+      </c>
+      <c r="M9" s="25"/>
+      <c r="N9" s="23">
+        <v>0.84750899999999996</v>
+      </c>
+      <c r="O9" s="23">
+        <v>0.82687500000000003</v>
+      </c>
+      <c r="P9" s="23">
+        <v>0.85707100000000003</v>
+      </c>
+      <c r="Q9" s="23">
+        <v>0.88927999999999996</v>
+      </c>
+      <c r="R9" s="21">
+        <v>13</v>
+      </c>
+      <c r="S9" s="25"/>
+      <c r="T9" s="23">
+        <v>0.86448400000000003</v>
+      </c>
+      <c r="U9" s="23">
+        <v>0.84282100000000004</v>
+      </c>
+      <c r="V9" s="23">
+        <v>0.85743100000000005</v>
+      </c>
+      <c r="W9" s="23">
+        <v>0.89017599999999997</v>
+      </c>
+      <c r="X9" s="21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0.9415</v>
+      </c>
+      <c r="H10" s="24"/>
+      <c r="I10" s="23">
+        <v>0.91649999999999998</v>
+      </c>
+      <c r="J10" s="23">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="K10" s="23">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="L10" s="27">
+        <v>15</v>
+      </c>
+      <c r="M10" s="25"/>
+      <c r="N10" s="23">
+        <v>0.91481900000000005</v>
+      </c>
+      <c r="O10" s="23">
+        <v>0.91885099999999997</v>
+      </c>
+      <c r="P10" s="23">
+        <v>0.92691500000000004</v>
+      </c>
+      <c r="Q10" s="23">
+        <v>0.92288300000000001</v>
+      </c>
+      <c r="R10" s="21">
+        <v>16</v>
+      </c>
+      <c r="S10" s="25"/>
+      <c r="T10" s="23">
+        <v>0.915493</v>
+      </c>
+      <c r="U10" s="23">
+        <v>0.91998000000000002</v>
+      </c>
+      <c r="V10" s="23">
+        <v>0.92652199999999996</v>
+      </c>
+      <c r="W10" s="23">
+        <v>0.92253499999999999</v>
+      </c>
+      <c r="X10" s="21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G11" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="H11" s="24"/>
+      <c r="I11" s="23">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="J11" s="23">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="K11" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="L11" s="27">
+        <v>13</v>
+      </c>
+      <c r="M11" s="25"/>
+      <c r="N11" s="23">
+        <v>0.91641499999999998</v>
+      </c>
+      <c r="O11" s="23">
+        <v>0.91742199999999996</v>
+      </c>
+      <c r="P11" s="23">
+        <v>0.918933</v>
+      </c>
+      <c r="Q11" s="23">
+        <v>0.91641499999999998</v>
+      </c>
+      <c r="R11" s="21">
+        <v>14</v>
+      </c>
+      <c r="S11" s="25"/>
+      <c r="T11" s="23">
+        <v>0.91586900000000004</v>
+      </c>
+      <c r="U11" s="23">
+        <v>0.91885099999999997</v>
+      </c>
+      <c r="V11" s="23">
+        <v>0.91985899999999998</v>
+      </c>
+      <c r="W11" s="23">
+        <v>0.91536499999999998</v>
+      </c>
+      <c r="X11" s="21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G12" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="H12" s="24"/>
+      <c r="I12" s="23">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="J12" s="23">
+        <v>0.90649999999999997</v>
+      </c>
+      <c r="K12" s="23">
+        <v>0.91</v>
+      </c>
+      <c r="L12" s="27">
+        <v>13</v>
+      </c>
+      <c r="M12" s="25"/>
+      <c r="N12" s="23">
+        <v>0.900756</v>
+      </c>
+      <c r="O12" s="23">
+        <v>0.90115999999999996</v>
+      </c>
+      <c r="P12" s="23">
+        <v>0.90267299999999995</v>
+      </c>
+      <c r="Q12" s="23">
+        <v>0.90932000000000002</v>
+      </c>
+      <c r="R12" s="21">
+        <v>17</v>
+      </c>
+      <c r="S12" s="25"/>
+      <c r="T12" s="23">
+        <v>0.90478599999999998</v>
+      </c>
+      <c r="U12" s="23">
+        <v>0.90221799999999996</v>
+      </c>
+      <c r="V12" s="23">
+        <v>0.89868999999999999</v>
+      </c>
+      <c r="W12" s="23">
+        <v>0.91234300000000002</v>
+      </c>
+      <c r="X12" s="21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G13" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="H13" s="24"/>
+      <c r="I13" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="J13" s="23">
+        <v>0.91549999999999998</v>
+      </c>
+      <c r="K13" s="23">
+        <v>0.91049999999999998</v>
+      </c>
+      <c r="L13" s="27">
+        <v>12</v>
+      </c>
+      <c r="M13" s="25"/>
+      <c r="N13" s="23">
+        <v>0.91444400000000003</v>
+      </c>
+      <c r="O13" s="23">
+        <v>0.91494699999999995</v>
+      </c>
+      <c r="P13" s="23">
+        <v>0.91595400000000005</v>
+      </c>
+      <c r="Q13" s="23">
+        <v>0.91041799999999995</v>
+      </c>
+      <c r="R13" s="21">
+        <v>13</v>
+      </c>
+      <c r="S13" s="25"/>
+      <c r="T13" s="23">
+        <v>0.91490400000000005</v>
+      </c>
+      <c r="U13" s="23">
+        <v>0.915408</v>
+      </c>
+      <c r="V13" s="23">
+        <v>0.91591100000000003</v>
+      </c>
+      <c r="W13" s="23">
+        <v>0.91037299999999999</v>
+      </c>
+      <c r="X13" s="21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G14" s="23">
+        <v>0.9415</v>
+      </c>
+      <c r="H14" s="24"/>
+      <c r="I14" s="23">
+        <v>0.89249999999999996</v>
+      </c>
+      <c r="J14" s="23">
+        <v>0.90049999999999997</v>
+      </c>
+      <c r="K14" s="23">
+        <v>0.91849999999999998</v>
+      </c>
+      <c r="L14" s="27">
+        <v>13</v>
+      </c>
+      <c r="M14" s="25"/>
+      <c r="N14" s="23">
+        <v>0.88525399999999999</v>
+      </c>
+      <c r="O14" s="23">
+        <v>0.89380999999999999</v>
+      </c>
+      <c r="P14" s="23">
+        <v>0.90286900000000003</v>
+      </c>
+      <c r="Q14" s="23">
+        <v>0.91897300000000004</v>
+      </c>
+      <c r="R14" s="21">
+        <v>13</v>
+      </c>
+      <c r="S14" s="25"/>
+      <c r="T14" s="23">
+        <v>0.89034199999999997</v>
+      </c>
+      <c r="U14" s="23">
+        <v>0.89738399999999996</v>
+      </c>
+      <c r="V14" s="23">
+        <v>0.90040200000000004</v>
+      </c>
+      <c r="W14" s="23">
+        <v>0.91851099999999997</v>
+      </c>
+      <c r="X14" s="21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="23">
+        <v>0.9415</v>
+      </c>
+      <c r="G15" s="23">
+        <v>0.93</v>
+      </c>
+      <c r="H15" s="24"/>
+      <c r="I15" s="23">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="J15" s="23">
+        <v>0.84950000000000003</v>
+      </c>
+      <c r="K15" s="23">
+        <v>0.88849999999999996</v>
+      </c>
+      <c r="L15" s="27">
+        <v>14</v>
+      </c>
+      <c r="M15" s="25"/>
+      <c r="N15" s="23">
+        <v>0.87361500000000003</v>
+      </c>
+      <c r="O15" s="23">
+        <v>0.86656599999999995</v>
+      </c>
+      <c r="P15" s="23">
+        <v>0.86807699999999999</v>
+      </c>
+      <c r="Q15" s="23">
+        <v>0.88922500000000004</v>
+      </c>
+      <c r="R15" s="21">
+        <v>14</v>
+      </c>
+      <c r="S15" s="25"/>
+      <c r="T15" s="23">
+        <v>0.87663599999999997</v>
+      </c>
+      <c r="U15" s="23">
+        <v>0.86448400000000003</v>
+      </c>
+      <c r="V15" s="23">
+        <v>0.86952099999999999</v>
+      </c>
+      <c r="W15" s="23">
+        <v>0.89174200000000003</v>
+      </c>
+      <c r="X15" s="21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="23">
+        <v>0.9415</v>
+      </c>
+      <c r="G16" s="23">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="23">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="J16" s="23">
+        <v>0.90349999999999997</v>
+      </c>
+      <c r="K16" s="23">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="L16" s="27">
+        <v>15</v>
+      </c>
+      <c r="M16" s="25"/>
+      <c r="N16" s="23">
+        <v>0.90529000000000004</v>
+      </c>
+      <c r="O16" s="23">
+        <v>0.90327500000000005</v>
+      </c>
+      <c r="P16" s="23">
+        <v>0.91335</v>
+      </c>
+      <c r="Q16" s="23">
+        <v>0.91133500000000001</v>
+      </c>
+      <c r="R16" s="21">
+        <v>15</v>
+      </c>
+      <c r="S16" s="25"/>
+      <c r="T16" s="23">
+        <v>0.90922800000000004</v>
+      </c>
+      <c r="U16" s="23">
+        <v>0.90317700000000001</v>
+      </c>
+      <c r="V16" s="23">
+        <v>0.913767</v>
+      </c>
+      <c r="W16" s="23">
+        <v>0.913767</v>
+      </c>
+      <c r="X16" s="21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="23">
+        <v>0.9415</v>
+      </c>
+      <c r="G17" s="23">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="23">
+        <v>0.80449999999999999</v>
+      </c>
+      <c r="J17" s="23">
+        <v>0.80549999999999999</v>
+      </c>
+      <c r="K17" s="23">
+        <v>0.879</v>
+      </c>
+      <c r="L17" s="27">
+        <v>18</v>
+      </c>
+      <c r="M17" s="25"/>
+      <c r="N17" s="23">
+        <v>0.86074700000000004</v>
+      </c>
+      <c r="O17" s="23">
+        <v>0.83299699999999999</v>
+      </c>
+      <c r="P17" s="23">
+        <v>0.86831499999999995</v>
+      </c>
+      <c r="Q17" s="23">
+        <v>0.87790100000000004</v>
+      </c>
+      <c r="R17" s="21">
+        <v>18</v>
+      </c>
+      <c r="S17" s="25"/>
+      <c r="T17" s="23">
+        <v>0.84793600000000002</v>
+      </c>
+      <c r="U17" s="23">
+        <v>0.81218500000000005</v>
+      </c>
+      <c r="V17" s="23">
+        <v>0.85901300000000003</v>
+      </c>
+      <c r="W17" s="23">
+        <v>0.88217500000000004</v>
+      </c>
+      <c r="X17" s="21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="23">
+        <v>0.9415</v>
+      </c>
+      <c r="G18" s="23">
+        <v>0.9415</v>
+      </c>
+      <c r="H18" s="24"/>
+      <c r="I18" s="23">
+        <v>0.9415</v>
+      </c>
+      <c r="J18" s="23">
+        <v>0.9415</v>
+      </c>
+      <c r="K18" s="23">
+        <v>0.94</v>
+      </c>
+      <c r="L18" s="27">
+        <v>12</v>
+      </c>
+      <c r="M18" s="25"/>
+      <c r="N18" s="23">
+        <v>0.94114699999999996</v>
+      </c>
+      <c r="O18" s="23">
+        <v>0.94064400000000004</v>
+      </c>
+      <c r="P18" s="23">
+        <v>0.94315899999999997</v>
+      </c>
+      <c r="Q18" s="23">
+        <v>0.940141</v>
+      </c>
+      <c r="R18" s="21">
+        <v>12</v>
+      </c>
+      <c r="S18" s="25"/>
+      <c r="T18" s="23">
+        <v>0.94114699999999996</v>
+      </c>
+      <c r="U18" s="23">
+        <v>0.94114699999999996</v>
+      </c>
+      <c r="V18" s="23">
+        <v>0.94315899999999997</v>
+      </c>
+      <c r="W18" s="23">
+        <v>0.93963799999999997</v>
+      </c>
+      <c r="X18" s="21">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I3:K3">
+    <cfRule type="top10" dxfId="63" priority="48" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:K4">
+    <cfRule type="top10" dxfId="62" priority="47" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:K5">
+    <cfRule type="top10" dxfId="61" priority="46" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:K6">
+    <cfRule type="top10" dxfId="60" priority="45" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:K7">
+    <cfRule type="top10" dxfId="59" priority="44" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8:K8">
+    <cfRule type="top10" dxfId="58" priority="43" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:K9">
+    <cfRule type="top10" dxfId="57" priority="42" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10:K10">
+    <cfRule type="top10" dxfId="56" priority="41" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:K11">
+    <cfRule type="top10" dxfId="55" priority="40" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:K12">
+    <cfRule type="top10" dxfId="54" priority="39" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:K13">
+    <cfRule type="top10" dxfId="53" priority="38" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:K14">
+    <cfRule type="top10" dxfId="52" priority="37" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:K15">
+    <cfRule type="top10" dxfId="51" priority="36" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:K16">
+    <cfRule type="top10" dxfId="50" priority="35" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17:K17">
+    <cfRule type="top10" dxfId="49" priority="34" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18:K18">
+    <cfRule type="top10" dxfId="48" priority="33" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:Q3">
+    <cfRule type="top10" dxfId="47" priority="32" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:Q4">
+    <cfRule type="top10" dxfId="46" priority="31" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5:Q5">
+    <cfRule type="top10" dxfId="45" priority="30" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6:Q6">
+    <cfRule type="top10" dxfId="44" priority="29" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:Q7">
+    <cfRule type="top10" dxfId="43" priority="28" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8:Q8">
+    <cfRule type="top10" dxfId="42" priority="27" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N9:Q9">
+    <cfRule type="top10" dxfId="41" priority="26" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N10:Q10">
+    <cfRule type="top10" dxfId="40" priority="25" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N11:Q11">
+    <cfRule type="top10" dxfId="39" priority="24" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N12:Q12">
+    <cfRule type="top10" dxfId="38" priority="23" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N13:Q13">
+    <cfRule type="top10" dxfId="37" priority="22" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N14:Q14">
+    <cfRule type="top10" dxfId="36" priority="21" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15:Q15">
+    <cfRule type="top10" dxfId="35" priority="20" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16:Q16">
+    <cfRule type="top10" dxfId="34" priority="19" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N17:Q17">
+    <cfRule type="top10" dxfId="33" priority="18" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N18:Q18">
+    <cfRule type="top10" dxfId="32" priority="17" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3:W3">
+    <cfRule type="top10" dxfId="15" priority="16" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4:W4">
+    <cfRule type="top10" dxfId="14" priority="15" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T5:W5">
+    <cfRule type="top10" dxfId="13" priority="14" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T6:W6">
+    <cfRule type="top10" dxfId="12" priority="13" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T7:W7">
+    <cfRule type="top10" dxfId="11" priority="12" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T8:W8">
+    <cfRule type="top10" dxfId="10" priority="11" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T9:W9">
+    <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T10:W10">
+    <cfRule type="top10" dxfId="8" priority="9" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T11:W11">
+    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T12:W12">
+    <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T13:W13">
+    <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T14:W14">
+    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T15:W15">
+    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T16:W16">
+    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T17:W17">
+    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T18:W18">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B1C7A9-35D6-3748-BB7B-2F2B565FF308}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2749,158 +6841,158 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C14:C17">
-    <cfRule type="top10" dxfId="95" priority="48" rank="1"/>
+    <cfRule type="top10" dxfId="207" priority="48" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:D17">
-    <cfRule type="top10" dxfId="94" priority="47" rank="1"/>
+    <cfRule type="top10" dxfId="206" priority="47" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E17">
-    <cfRule type="top10" dxfId="93" priority="46" rank="1"/>
+    <cfRule type="top10" dxfId="205" priority="46" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F17">
-    <cfRule type="top10" dxfId="92" priority="45" rank="1"/>
+    <cfRule type="top10" dxfId="204" priority="45" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:G17">
-    <cfRule type="top10" dxfId="91" priority="44" rank="1"/>
+    <cfRule type="top10" dxfId="203" priority="44" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:H17">
-    <cfRule type="top10" dxfId="90" priority="43" rank="1"/>
+    <cfRule type="top10" dxfId="202" priority="43" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:I17">
-    <cfRule type="top10" dxfId="89" priority="42" rank="1"/>
+    <cfRule type="top10" dxfId="201" priority="42" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:J17">
-    <cfRule type="top10" dxfId="88" priority="41" rank="1"/>
+    <cfRule type="top10" dxfId="200" priority="41" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:K17">
-    <cfRule type="top10" dxfId="87" priority="40" rank="1"/>
+    <cfRule type="top10" dxfId="199" priority="40" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14:L17">
-    <cfRule type="top10" dxfId="86" priority="39" rank="1"/>
+    <cfRule type="top10" dxfId="198" priority="39" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14:M17">
-    <cfRule type="top10" dxfId="85" priority="38" rank="1"/>
+    <cfRule type="top10" dxfId="197" priority="38" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14:N17">
-    <cfRule type="top10" dxfId="84" priority="37" rank="1"/>
+    <cfRule type="top10" dxfId="196" priority="37" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O14:O17">
-    <cfRule type="top10" dxfId="83" priority="36" rank="1"/>
+    <cfRule type="top10" dxfId="195" priority="36" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P14:P17">
-    <cfRule type="top10" dxfId="82" priority="35" rank="1"/>
+    <cfRule type="top10" dxfId="194" priority="35" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:Q17">
-    <cfRule type="top10" dxfId="81" priority="34" rank="1"/>
+    <cfRule type="top10" dxfId="193" priority="34" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:R17">
-    <cfRule type="top10" dxfId="80" priority="33" rank="1"/>
+    <cfRule type="top10" dxfId="192" priority="33" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:C23">
-    <cfRule type="top10" dxfId="79" priority="32" rank="1"/>
+    <cfRule type="top10" dxfId="191" priority="32" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:D23">
-    <cfRule type="top10" dxfId="78" priority="31" rank="1"/>
+    <cfRule type="top10" dxfId="190" priority="31" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E23">
-    <cfRule type="top10" dxfId="77" priority="30" rank="1"/>
+    <cfRule type="top10" dxfId="189" priority="30" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F23">
-    <cfRule type="top10" dxfId="76" priority="29" rank="1"/>
+    <cfRule type="top10" dxfId="188" priority="29" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:G23">
-    <cfRule type="top10" dxfId="75" priority="28" rank="1"/>
+    <cfRule type="top10" dxfId="187" priority="28" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:H23">
-    <cfRule type="top10" dxfId="74" priority="27" rank="1"/>
+    <cfRule type="top10" dxfId="186" priority="27" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I23">
-    <cfRule type="top10" dxfId="73" priority="26" rank="1"/>
+    <cfRule type="top10" dxfId="185" priority="26" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:J23">
-    <cfRule type="top10" dxfId="72" priority="25" rank="1"/>
+    <cfRule type="top10" dxfId="184" priority="25" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:K23">
-    <cfRule type="top10" dxfId="71" priority="24" rank="1"/>
+    <cfRule type="top10" dxfId="183" priority="24" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:L23">
-    <cfRule type="top10" dxfId="70" priority="23" rank="1"/>
+    <cfRule type="top10" dxfId="182" priority="23" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M20:M23">
-    <cfRule type="top10" dxfId="69" priority="22" rank="1"/>
+    <cfRule type="top10" dxfId="181" priority="22" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:N23">
-    <cfRule type="top10" dxfId="68" priority="21" rank="1"/>
+    <cfRule type="top10" dxfId="180" priority="21" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O20:O23">
-    <cfRule type="top10" dxfId="67" priority="20" rank="1"/>
+    <cfRule type="top10" dxfId="179" priority="20" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20:P23">
-    <cfRule type="top10" dxfId="66" priority="19" rank="1"/>
+    <cfRule type="top10" dxfId="178" priority="19" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q20:Q23">
-    <cfRule type="top10" dxfId="65" priority="18" rank="1"/>
+    <cfRule type="top10" dxfId="177" priority="18" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R20:R23">
-    <cfRule type="top10" dxfId="64" priority="17" rank="1"/>
+    <cfRule type="top10" dxfId="176" priority="17" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:C11">
-    <cfRule type="top10" dxfId="63" priority="16" rank="1"/>
+    <cfRule type="top10" dxfId="175" priority="16" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D11">
-    <cfRule type="top10" dxfId="62" priority="15" rank="1"/>
+    <cfRule type="top10" dxfId="174" priority="15" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E11">
-    <cfRule type="top10" dxfId="61" priority="14" rank="1"/>
+    <cfRule type="top10" dxfId="173" priority="14" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F11">
-    <cfRule type="top10" dxfId="60" priority="13" rank="1"/>
+    <cfRule type="top10" dxfId="172" priority="13" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:G11">
-    <cfRule type="top10" dxfId="59" priority="12" rank="1"/>
+    <cfRule type="top10" dxfId="171" priority="12" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H11">
-    <cfRule type="top10" dxfId="58" priority="11" rank="1"/>
+    <cfRule type="top10" dxfId="170" priority="11" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I11">
-    <cfRule type="top10" dxfId="57" priority="10" rank="1"/>
+    <cfRule type="top10" dxfId="169" priority="10" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:J11">
-    <cfRule type="top10" dxfId="56" priority="9" rank="1"/>
+    <cfRule type="top10" dxfId="168" priority="9" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:K11">
-    <cfRule type="top10" dxfId="55" priority="8" rank="1"/>
+    <cfRule type="top10" dxfId="167" priority="8" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:L11">
-    <cfRule type="top10" dxfId="54" priority="7" rank="1"/>
+    <cfRule type="top10" dxfId="166" priority="7" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9:M11">
-    <cfRule type="top10" dxfId="53" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="165" priority="6" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:N11">
-    <cfRule type="top10" dxfId="52" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="164" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9:O11">
-    <cfRule type="top10" dxfId="51" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="163" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9:P11">
-    <cfRule type="top10" dxfId="50" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="162" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q9:Q11">
-    <cfRule type="top10" dxfId="49" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="161" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R9:R11">
-    <cfRule type="top10" dxfId="48" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="160" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4214CDF2-8188-D948-ADD3-2E44AA60B30B}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -3984,154 +8076,154 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N3:Q3">
-    <cfRule type="top10" dxfId="47" priority="48" rank="1"/>
+    <cfRule type="top10" dxfId="159" priority="48" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:Q4">
-    <cfRule type="top10" dxfId="46" priority="47" rank="1"/>
+    <cfRule type="top10" dxfId="158" priority="47" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:Q5">
-    <cfRule type="top10" dxfId="45" priority="46" rank="1"/>
+    <cfRule type="top10" dxfId="157" priority="46" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:Q6">
-    <cfRule type="top10" dxfId="44" priority="45" rank="1"/>
+    <cfRule type="top10" dxfId="156" priority="45" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:Q7">
-    <cfRule type="top10" dxfId="43" priority="44" rank="1"/>
+    <cfRule type="top10" dxfId="155" priority="44" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:Q8">
-    <cfRule type="top10" dxfId="42" priority="43" rank="1"/>
+    <cfRule type="top10" dxfId="154" priority="43" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:Q9">
-    <cfRule type="top10" dxfId="41" priority="42" rank="1"/>
+    <cfRule type="top10" dxfId="153" priority="42" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10:Q10">
-    <cfRule type="top10" dxfId="40" priority="41" rank="1"/>
+    <cfRule type="top10" dxfId="152" priority="41" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11:Q11">
-    <cfRule type="top10" dxfId="39" priority="40" rank="1"/>
+    <cfRule type="top10" dxfId="151" priority="40" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12:Q12">
-    <cfRule type="top10" dxfId="38" priority="39" rank="1"/>
+    <cfRule type="top10" dxfId="150" priority="39" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13:Q13">
-    <cfRule type="top10" dxfId="37" priority="38" rank="1"/>
+    <cfRule type="top10" dxfId="149" priority="38" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14:Q14">
-    <cfRule type="top10" dxfId="36" priority="37" rank="1"/>
+    <cfRule type="top10" dxfId="148" priority="37" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:Q15">
-    <cfRule type="top10" dxfId="35" priority="36" rank="1"/>
+    <cfRule type="top10" dxfId="147" priority="36" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16:Q16">
-    <cfRule type="top10" dxfId="34" priority="35" rank="1"/>
+    <cfRule type="top10" dxfId="146" priority="35" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17:Q17">
-    <cfRule type="top10" dxfId="33" priority="34" rank="1"/>
+    <cfRule type="top10" dxfId="145" priority="34" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:Q18">
-    <cfRule type="top10" dxfId="32" priority="33" rank="1"/>
+    <cfRule type="top10" dxfId="144" priority="33" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:W3">
-    <cfRule type="top10" dxfId="31" priority="32" rank="1"/>
+    <cfRule type="top10" dxfId="143" priority="32" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:W4">
-    <cfRule type="top10" dxfId="30" priority="31" rank="1"/>
+    <cfRule type="top10" dxfId="142" priority="31" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:W5">
-    <cfRule type="top10" dxfId="29" priority="30" rank="1"/>
+    <cfRule type="top10" dxfId="141" priority="30" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6:W6">
-    <cfRule type="top10" dxfId="28" priority="29" rank="1"/>
+    <cfRule type="top10" dxfId="140" priority="29" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T7:W7">
-    <cfRule type="top10" dxfId="27" priority="28" rank="1"/>
+    <cfRule type="top10" dxfId="139" priority="28" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T8:W8">
-    <cfRule type="top10" dxfId="26" priority="27" rank="1"/>
+    <cfRule type="top10" dxfId="138" priority="27" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T9:W9">
-    <cfRule type="top10" dxfId="25" priority="26" rank="1"/>
+    <cfRule type="top10" dxfId="137" priority="26" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T10:W10">
-    <cfRule type="top10" dxfId="24" priority="25" rank="1"/>
+    <cfRule type="top10" dxfId="136" priority="25" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T11:W11">
-    <cfRule type="top10" dxfId="23" priority="24" rank="1"/>
+    <cfRule type="top10" dxfId="135" priority="24" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T12:W12">
-    <cfRule type="top10" dxfId="22" priority="23" rank="1"/>
+    <cfRule type="top10" dxfId="134" priority="23" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T13:W13">
-    <cfRule type="top10" dxfId="21" priority="22" rank="1"/>
+    <cfRule type="top10" dxfId="133" priority="22" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T14:W14">
-    <cfRule type="top10" dxfId="20" priority="21" rank="1"/>
+    <cfRule type="top10" dxfId="132" priority="21" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T15:W15">
-    <cfRule type="top10" dxfId="19" priority="20" rank="1"/>
+    <cfRule type="top10" dxfId="131" priority="20" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:W16">
-    <cfRule type="top10" dxfId="18" priority="19" rank="1"/>
+    <cfRule type="top10" dxfId="130" priority="19" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T17:W17">
-    <cfRule type="top10" dxfId="17" priority="18" rank="1"/>
+    <cfRule type="top10" dxfId="129" priority="18" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T18:W18">
-    <cfRule type="top10" dxfId="16" priority="17" rank="1"/>
+    <cfRule type="top10" dxfId="128" priority="17" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:K3">
-    <cfRule type="top10" dxfId="15" priority="16" rank="1"/>
+    <cfRule type="top10" dxfId="127" priority="16" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:K4">
-    <cfRule type="top10" dxfId="14" priority="15" rank="1"/>
+    <cfRule type="top10" dxfId="126" priority="15" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:K5">
-    <cfRule type="top10" dxfId="13" priority="14" rank="1"/>
+    <cfRule type="top10" dxfId="125" priority="14" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:K6">
-    <cfRule type="top10" dxfId="12" priority="13" rank="1"/>
+    <cfRule type="top10" dxfId="124" priority="13" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:K7">
-    <cfRule type="top10" dxfId="11" priority="12" rank="1"/>
+    <cfRule type="top10" dxfId="123" priority="12" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:K8">
-    <cfRule type="top10" dxfId="10" priority="11" rank="1"/>
+    <cfRule type="top10" dxfId="122" priority="11" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:K9">
-    <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
+    <cfRule type="top10" dxfId="121" priority="10" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:K10">
-    <cfRule type="top10" dxfId="8" priority="9" rank="1"/>
+    <cfRule type="top10" dxfId="120" priority="9" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:K11">
-    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
+    <cfRule type="top10" dxfId="119" priority="8" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:K12">
-    <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
+    <cfRule type="top10" dxfId="118" priority="7" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:K13">
-    <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="117" priority="6" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:K14">
-    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="116" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:K15">
-    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="115" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:K16">
-    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="114" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:K17">
-    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="113" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:K18">
-    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="112" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732572F4-7426-2643-8547-30B6090A3AB1}">
   <dimension ref="A1:R32"/>
   <sheetViews>

</xml_diff>